<commit_message>
update the latest configuration files
</commit_message>
<xml_diff>
--- a/courses/excel/onshore/coe/aibt/promotions/BESPOKE_GRAMMAR_SCHOOL_OF_ENGLISH.xlsx
+++ b/courses/excel/onshore/coe/aibt/promotions/BESPOKE_GRAMMAR_SCHOOL_OF_ENGLISH.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zelon\Documents\Brochure APP\documents\new version\onshore\coe\aibt\promotions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aibtaus-my.sharepoint.com/personal/f_zhang_aibtglobal_edu_au/Documents/App for VC/excel table template/courses/courses/excel/offshore/SEAPAE/aibt/promotions/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="21" documentId="11_C90BF2A8750F73CF3F04193D4A9DBCF4AFE1CC54" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FBB92BA-CE2D-410E-9D11-44263ECDF31F}"/>
   <bookViews>
-    <workbookView xWindow="1935" yWindow="-105" windowWidth="22140" windowHeight="13170"/>
+    <workbookView xWindow="-19290" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="courses" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>vetCode</t>
   </si>
@@ -44,19 +45,42 @@
     <t>durationDetail</t>
   </si>
   <si>
-    <t>offshoreTuition</t>
-  </si>
-  <si>
-    <t>onshoreTuition</t>
-  </si>
-  <si>
     <t>location</t>
   </si>
   <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>NSW/QLD/TAS</t>
+    <t>tuition</t>
+  </si>
+  <si>
+    <t>durationMin</t>
+  </si>
+  <si>
+    <t>durationMax</t>
+  </si>
+  <si>
+    <t>tuitionDetail</t>
+  </si>
+  <si>
+    <t>tuitionHalf</t>
+  </si>
+  <si>
+    <t>tuitionHalfDetail</t>
+  </si>
+  <si>
+    <t>locationDetail</t>
+  </si>
+  <si>
+    <t>placementDuration</t>
+  </si>
+  <si>
+    <t>placementFee</t>
+  </si>
+  <si>
+    <t>placementDetail</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>promotionValidity</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">General English (Beginner to Upper Intermediate) - ELICOS only </t>
@@ -65,50 +89,44 @@
     <t>General English (Beginner to Upper Intermediate) - packaged with any other VET course</t>
   </si>
   <si>
-    <t>(Minimum of 10 Weeks)</t>
-  </si>
-  <si>
-    <t>(Minimum of 10 Weeks)
-Students will receive the
-first 10 weeks of ELICOS
-FREE. If the duration
-of ELICOS within the
-package is greater than
-10 weeks, the remaining
-duration of ELICOS will be
-$185 per week</t>
+    <t>089486D</t>
+  </si>
+  <si>
+    <t>BESPOKE GRAMMAR SCHOOL OF ENGLISH</t>
+  </si>
+  <si>
+    <t>10 weeks</t>
+  </si>
+  <si>
+    <t>First 10 weeks</t>
   </si>
   <si>
     <t>185/week
 1,850 total</t>
   </si>
   <si>
-    <t>Free (if ELICOS duration is greater than 10 weeks, the remaining duration of ELICOS will be 185/week)</t>
+    <t>Free</t>
+  </si>
+  <si>
+    <t>if ELICOS duration is greater than 10 weeks, the remaining duration of ELICOS will be 185/week</t>
+  </si>
+  <si>
+    <t>Promotion valid until  31th Dec 2021</t>
+  </si>
+  <si>
+    <t>NSW/QLD/TAS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -117,6 +135,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -139,23 +165,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -436,86 +455,140 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="73.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="19.5" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="14.42578125" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:18" ht="20.100000000000001" customHeight="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>10</v>
+    <row r="2" spans="1:18" ht="45">
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>10</v>
+    <row r="3" spans="1:18" ht="120">
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>